<commit_message>
Group A weekend, Group BWeekday, Group B Weekend added but potentially found an error in code
</commit_message>
<xml_diff>
--- a/Results/VisitFreqResults.xlsx
+++ b/Results/VisitFreqResults.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ellieodole/Desktop/CompEpi/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B2B98B4-A0DC-B244-8EB9-B1D3F4FBA913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFDE0FFB-11FC-5247-85C6-971FB5B33421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12040" yWindow="500" windowWidth="16760" windowHeight="15800" activeTab="1" xr2:uid="{79939B0F-1E38-4E44-BCA6-B963B8C4AFB2}"/>
+    <workbookView xWindow="12040" yWindow="500" windowWidth="16760" windowHeight="15800" activeTab="4" xr2:uid="{79939B0F-1E38-4E44-BCA6-B963B8C4AFB2}"/>
   </bookViews>
   <sheets>
     <sheet name="GroupA Weekday" sheetId="1" r:id="rId1"/>
     <sheet name="GroupA Weekend" sheetId="2" r:id="rId2"/>
+    <sheet name="GroupB Weekday" sheetId="3" r:id="rId3"/>
+    <sheet name="GroupB Weekend" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="9">
   <si>
     <t>Job Type ID</t>
   </si>
@@ -56,6 +59,12 @@
   </si>
   <si>
     <t>NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21 28 29 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">21 29 </t>
   </si>
 </sst>
 </file>
@@ -410,7 +419,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A34"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -903,8 +912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4746EA15-A9C7-214F-9C01-6BD036FBC0AB}">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -930,76 +939,211 @@
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>1.1305270000000001</v>
+      </c>
+      <c r="D2">
+        <v>1.802E-3</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>0.88156000000000001</v>
+      </c>
+      <c r="D3">
+        <v>1.704E-2</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>1.0830869999999999</v>
+      </c>
+      <c r="D4">
+        <v>6.3379999999999999E-3</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>0.69742999999999999</v>
+      </c>
+      <c r="D6">
+        <v>1.583E-2</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>0.73680000000000001</v>
+      </c>
+      <c r="D7">
+        <v>1.14E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>1.1997370000000001</v>
+      </c>
+      <c r="D8">
+        <v>3.0360000000000001E-3</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>0.61319999999999997</v>
+      </c>
+      <c r="D9">
+        <v>0.9456</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>0.86224299999999998</v>
+      </c>
+      <c r="D11">
+        <v>5.6360000000000004E-3</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>0.88705999999999996</v>
+      </c>
+      <c r="D12">
+        <v>1.0070000000000001E-2</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>0.45472000000000001</v>
+      </c>
+      <c r="D13">
+        <v>2.0160000000000001E-2</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
+      <c r="B14">
+        <v>29</v>
+      </c>
+      <c r="C14">
+        <v>1.31172</v>
+      </c>
+      <c r="D14">
+        <v>1.111E-2</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>0.80020000000000002</v>
+      </c>
+      <c r="D15">
+        <v>1.5900000000000001E-2</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>0.27417000000000002</v>
+      </c>
+      <c r="D16">
+        <v>5.2769999999999997E-2</v>
+      </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17">
@@ -1094,4 +1238,875 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{068B7771-B725-FB42-856E-28518367850A}">
+  <dimension ref="A1:D34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>0.63712500000000005</v>
+      </c>
+      <c r="D2">
+        <v>3.5530000000000002E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>0.73249900000000001</v>
+      </c>
+      <c r="D15">
+        <v>4.6319999999999998E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>6</v>
+      </c>
+      <c r="C21">
+        <v>0.28042</v>
+      </c>
+      <c r="D21">
+        <v>1.0789999999999999E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>6</v>
+      </c>
+      <c r="C31">
+        <v>0.50468800000000003</v>
+      </c>
+      <c r="D31">
+        <v>8.6020000000000003E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22F9972F-BD45-624B-83B7-904B12FD1F4C}">
+  <dimension ref="A1:D34"/>
+  <sheetViews>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:D34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>-1.2346999999999999</v>
+      </c>
+      <c r="D2">
+        <v>0.12509999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>-1.5764</v>
+      </c>
+      <c r="D15">
+        <v>0.23860000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F921510E-5ECC-824C-8A83-1A620A33756A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the results further and wrote script to make graphics for comparison
</commit_message>
<xml_diff>
--- a/Results/VisitFreqResults.xlsx
+++ b/Results/VisitFreqResults.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ellieodole/Desktop/CompEpi/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFDE0FFB-11FC-5247-85C6-971FB5B33421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C0322F-5FBB-D346-B457-87F64DE71D1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12040" yWindow="500" windowWidth="16760" windowHeight="15800" activeTab="4" xr2:uid="{79939B0F-1E38-4E44-BCA6-B963B8C4AFB2}"/>
+    <workbookView xWindow="340" yWindow="560" windowWidth="16760" windowHeight="15800" activeTab="3" xr2:uid="{79939B0F-1E38-4E44-BCA6-B963B8C4AFB2}"/>
   </bookViews>
   <sheets>
     <sheet name="GroupA Weekday" sheetId="1" r:id="rId1"/>
     <sheet name="GroupA Weekend" sheetId="2" r:id="rId2"/>
     <sheet name="GroupB Weekday" sheetId="3" r:id="rId3"/>
     <sheet name="GroupB Weekend" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet3" sheetId="5" r:id="rId5"/>
+    <sheet name="GroupC Weekday " sheetId="5" r:id="rId5"/>
+    <sheet name="GroupC Weekend" sheetId="6" r:id="rId6"/>
+    <sheet name="GroupD Weekday" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="14">
   <si>
     <t>Job Type ID</t>
   </si>
@@ -65,6 +67,21 @@
   </si>
   <si>
     <t xml:space="preserve">21 29 </t>
+  </si>
+  <si>
+    <t>22 38 41</t>
+  </si>
+  <si>
+    <t>38 41</t>
+  </si>
+  <si>
+    <t>22 38</t>
+  </si>
+  <si>
+    <t>22 41</t>
+  </si>
+  <si>
+    <t>33 37 42</t>
   </si>
 </sst>
 </file>
@@ -1735,8 +1752,374 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22F9972F-BD45-624B-83B7-904B12FD1F4C}">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:D34"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>-1.2346999999999999</v>
+      </c>
+      <c r="D2">
+        <v>0.12509999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>-1.5764</v>
+      </c>
+      <c r="D15">
+        <v>0.23860000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F921510E-5ECC-824C-8A83-1A620A33756A}">
+  <dimension ref="A1:D34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1759,14 +2142,14 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>6</v>
+      <c r="B2" t="s">
+        <v>9</v>
       </c>
       <c r="C2">
-        <v>-1.2346999999999999</v>
+        <v>1.0176398</v>
       </c>
       <c r="D2">
-        <v>0.12509999999999999</v>
+        <v>9.8090000000000004E-4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1774,13 +2157,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>0.70259300000000002</v>
+      </c>
+      <c r="D3">
+        <v>7.319E-3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1788,13 +2171,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>1.1000300000000001</v>
+      </c>
+      <c r="D4">
+        <v>5.7299999999999999E-3</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1802,13 +2185,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>6.8140000000000006E-2</v>
+      </c>
+      <c r="D5">
+        <v>2.1533E-2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1816,13 +2199,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>0.50975000000000004</v>
+      </c>
+      <c r="D6">
+        <v>1.533E-2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1830,13 +2213,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>0.61938000000000004</v>
+      </c>
+      <c r="D7">
+        <v>3.8300000000000001E-3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1844,13 +2227,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>1.049318</v>
+      </c>
+      <c r="D8">
+        <v>1.688E-3</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1858,13 +2241,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>0.54871999999999999</v>
+      </c>
+      <c r="D9">
+        <v>1.1339999999999999E-2</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -1872,13 +2255,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>0.52502599999999999</v>
+      </c>
+      <c r="D10">
+        <v>9.7579999999999993E-3</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1886,13 +2269,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>0.95747499999999997</v>
+      </c>
+      <c r="D11">
+        <v>3.075E-3</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -1900,13 +2283,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" t="s">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>1.3028409999999999</v>
+      </c>
+      <c r="D12">
+        <v>6.6270000000000001E-3</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -1914,13 +2297,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="C13">
+        <v>0.13996500000000001</v>
+      </c>
+      <c r="D13">
+        <v>9.7730000000000004E-3</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1928,27 +2311,27 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <v>1.08253</v>
+      </c>
+      <c r="D14">
+        <v>8.7270000000000004E-3</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15">
-        <v>6</v>
+      <c r="B15" t="s">
+        <v>11</v>
       </c>
       <c r="C15">
-        <v>-1.5764</v>
+        <v>0.42160999999999998</v>
       </c>
       <c r="D15">
-        <v>0.23860000000000001</v>
+        <v>0.1111</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1956,13 +2339,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="C16">
+        <v>0.27840999999999999</v>
+      </c>
+      <c r="D16">
+        <v>2.1360000000000001E-2</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -1970,13 +2353,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" t="s">
-        <v>6</v>
+        <v>11</v>
+      </c>
+      <c r="C17">
+        <v>-0.1004</v>
+      </c>
+      <c r="D17">
+        <v>0.10539999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -1984,13 +2367,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="C18">
+        <v>1.1253660000000001</v>
+      </c>
+      <c r="D18">
+        <v>4.6010000000000001E-3</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -1998,27 +2381,27 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" t="s">
-        <v>6</v>
+        <v>11</v>
+      </c>
+      <c r="C19">
+        <v>0.61845000000000006</v>
+      </c>
+      <c r="D19">
+        <v>1.5219999999999999E-2</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" t="s">
-        <v>6</v>
+      <c r="B20">
+        <v>38</v>
+      </c>
+      <c r="C20">
+        <v>6.9970000000000004E-2</v>
+      </c>
+      <c r="D20">
+        <v>6.4839999999999995E-2</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -2026,72 +2409,195 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>6</v>
+        <v>22</v>
+      </c>
+      <c r="C21">
+        <v>0.70640199999999997</v>
+      </c>
+      <c r="D21">
+        <v>8.7489999999999998E-3</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
+      <c r="B22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22">
+        <v>0.27207999999999999</v>
+      </c>
+      <c r="D22">
+        <v>3.3750000000000002E-2</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
+      <c r="B24">
+        <v>22</v>
+      </c>
+      <c r="C24">
+        <v>-0.14329</v>
+      </c>
+      <c r="D24">
+        <v>4.7210000000000002E-2</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
+      <c r="B26">
+        <v>41</v>
+      </c>
+      <c r="C26">
+        <v>1.2818400000000001</v>
+      </c>
+      <c r="D26">
+        <v>2.1510000000000001E-2</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27">
+        <v>0.45272000000000001</v>
+      </c>
+      <c r="D27">
+        <v>2.1139999999999999E-2</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
+      <c r="B28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28">
+        <v>0.39456000000000002</v>
+      </c>
+      <c r="D28">
+        <v>5.2639999999999999E-2</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
+      <c r="B30">
+        <v>22</v>
+      </c>
+      <c r="C30">
+        <v>-0.38603999999999999</v>
+      </c>
+      <c r="D30">
+        <v>4.6870000000000002E-2</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
+      <c r="B31">
+        <v>22</v>
+      </c>
+      <c r="C31">
+        <v>0.15654999999999999</v>
+      </c>
+      <c r="D31">
+        <v>3.9140000000000001E-2</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32">
+        <v>0.80215700000000001</v>
+      </c>
+      <c r="D32">
+        <v>5.078E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33">
+        <v>0.46140399999999998</v>
+      </c>
+      <c r="D33">
+        <v>9.0830000000000008E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34">
+        <v>0.17180000000000001</v>
+      </c>
+      <c r="D34">
+        <v>3.7900000000000003E-2</v>
       </c>
     </row>
   </sheetData>
@@ -2099,14 +2605,759 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F921510E-5ECC-824C-8A83-1A620A33756A}">
-  <dimension ref="A1"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3554EACD-3F4E-5E4B-81F7-35DD23FF1BC3}">
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2">
+        <v>1.039409</v>
+      </c>
+      <c r="D2">
+        <v>1.6429999999999999E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>0.78441000000000005</v>
+      </c>
+      <c r="D3">
+        <v>1.5720000000000001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>1.12565</v>
+      </c>
+      <c r="D4">
+        <v>9.6439999999999998E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>0.33539000000000002</v>
+      </c>
+      <c r="D5">
+        <v>9.1429999999999997E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>0.61380999999999997</v>
+      </c>
+      <c r="D6">
+        <v>0.36330000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>0.743093</v>
+      </c>
+      <c r="D7">
+        <v>6.2290000000000002E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>1.079847</v>
+      </c>
+      <c r="D8">
+        <v>2.764E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9">
+        <v>1.00237</v>
+      </c>
+      <c r="D9">
+        <v>2.1950000000000001E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>0.59606999999999999</v>
+      </c>
+      <c r="D10">
+        <v>1.7940000000000001E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>0.96724500000000002</v>
+      </c>
+      <c r="D11">
+        <v>5.6049999999999997E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>1.34687</v>
+      </c>
+      <c r="D12">
+        <v>1.059E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13">
+        <v>0.3306</v>
+      </c>
+      <c r="D13">
+        <v>3.0300000000000001E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <v>1.0972999999999999</v>
+      </c>
+      <c r="D14">
+        <v>1.5559999999999999E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15">
+        <v>0.44923999999999997</v>
+      </c>
+      <c r="D15">
+        <v>1.941E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16">
+        <v>0.40766000000000002</v>
+      </c>
+      <c r="D16">
+        <v>3.6290000000000003E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18">
+        <v>1.1438900000000001</v>
+      </c>
+      <c r="D18">
+        <v>8.3199999999999993E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19">
+        <v>0.59543999999999997</v>
+      </c>
+      <c r="D19">
+        <v>3.1660000000000001E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>22</v>
+      </c>
+      <c r="C21">
+        <v>0.75436000000000003</v>
+      </c>
+      <c r="D21">
+        <v>1.4239999999999999E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22">
+        <v>0.72341</v>
+      </c>
+      <c r="D22">
+        <v>7.2239999999999999E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>22</v>
+      </c>
+      <c r="C24">
+        <v>-8.8830000000000006E-2</v>
+      </c>
+      <c r="D24">
+        <v>0.14893000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>41</v>
+      </c>
+      <c r="C26">
+        <v>1.2939499999999999</v>
+      </c>
+      <c r="D26">
+        <v>3.5189999999999999E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27">
+        <v>0.68291000000000002</v>
+      </c>
+      <c r="D27">
+        <v>7.0580000000000004E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>41</v>
+      </c>
+      <c r="C28">
+        <v>0.45895999999999998</v>
+      </c>
+      <c r="D28">
+        <v>8.4159999999999999E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>22</v>
+      </c>
+      <c r="C30">
+        <v>-0.27110000000000001</v>
+      </c>
+      <c r="D30">
+        <v>0.1012</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32">
+        <v>0.92107799999999995</v>
+      </c>
+      <c r="D32">
+        <v>8.2470000000000009E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33">
+        <v>0.51402999999999999</v>
+      </c>
+      <c r="D33">
+        <v>1.405E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34">
+        <v>0.62019000000000002</v>
+      </c>
+      <c r="D34">
+        <v>6.4140000000000003E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A710AF1E-AAF0-554A-A227-651F57756BEE}">
+  <dimension ref="A1:D34"/>
+  <sheetViews>
+    <sheetView zoomScale="134" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2">
+        <v>0.92041899999999999</v>
+      </c>
+      <c r="D2">
+        <v>1.384E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <v>0.68167999999999995</v>
+      </c>
+      <c r="D3">
+        <v>1.162E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4">
+        <v>1.021434</v>
+      </c>
+      <c r="D4">
+        <v>4.7660000000000003E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>4.4359999999999997E-2</v>
+      </c>
+      <c r="D5">
+        <v>2.1600000000000001E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>0.75766</v>
+      </c>
+      <c r="D6">
+        <v>1.847E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>0.496979</v>
+      </c>
+      <c r="D7">
+        <v>5.385E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8">
+        <v>1.0889120000000001</v>
+      </c>
+      <c r="D8">
+        <v>2.0330000000000001E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9">
+        <v>0.32496999999999998</v>
+      </c>
+      <c r="D9">
+        <v>1.7239999999999998E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated graphics and got through Vist Freq D Weekday
</commit_message>
<xml_diff>
--- a/Results/VisitFreqResults.xlsx
+++ b/Results/VisitFreqResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ellieodole/Desktop/CompEpi/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C0322F-5FBB-D346-B457-87F64DE71D1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B5BF80B-3C8C-284F-8C2D-27F5514FC5DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="560" windowWidth="16760" windowHeight="15800" activeTab="3" xr2:uid="{79939B0F-1E38-4E44-BCA6-B963B8C4AFB2}"/>
+    <workbookView xWindow="12040" yWindow="500" windowWidth="16760" windowHeight="15800" firstSheet="3" activeTab="7" xr2:uid="{79939B0F-1E38-4E44-BCA6-B963B8C4AFB2}"/>
   </bookViews>
   <sheets>
     <sheet name="GroupA Weekday" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,8 @@
     <sheet name="GroupC Weekday " sheetId="5" r:id="rId5"/>
     <sheet name="GroupC Weekend" sheetId="6" r:id="rId6"/>
     <sheet name="GroupD Weekday" sheetId="7" r:id="rId7"/>
+    <sheet name="GroupD Weekend" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet2" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="17">
   <si>
     <t>Job Type ID</t>
   </si>
@@ -82,6 +84,15 @@
   </si>
   <si>
     <t>33 37 42</t>
+  </si>
+  <si>
+    <t>37 42</t>
+  </si>
+  <si>
+    <t>33 37</t>
+  </si>
+  <si>
+    <t>33 42</t>
   </si>
 </sst>
 </file>
@@ -1752,7 +1763,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22F9972F-BD45-624B-83B7-904B12FD1F4C}">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -3100,8 +3113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A710AF1E-AAF0-554A-A227-651F57756BEE}">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView zoomScale="134" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView topLeftCell="A14" zoomScale="134" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3236,6 +3249,727 @@
       <c r="A10">
         <v>9</v>
       </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10">
+        <v>0.20016999999999999</v>
+      </c>
+      <c r="D10">
+        <v>1.3129999999999999E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11">
+        <v>0.94286099999999995</v>
+      </c>
+      <c r="D11">
+        <v>4.7369999999999999E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12">
+        <v>0.96446600000000005</v>
+      </c>
+      <c r="D12">
+        <v>7.3140000000000002E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13">
+        <v>0.38978000000000002</v>
+      </c>
+      <c r="D13">
+        <v>1.3610000000000001E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>1.0888279999999999</v>
+      </c>
+      <c r="D14">
+        <v>8.0909999999999992E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <v>0.60887899999999995</v>
+      </c>
+      <c r="D15">
+        <v>4.3779999999999999E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16">
+        <v>0.32774999999999999</v>
+      </c>
+      <c r="D16">
+        <v>2.8979999999999999E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17">
+        <v>-0.21959999999999999</v>
+      </c>
+      <c r="D17">
+        <v>0.12770000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18">
+        <v>0.34823999999999999</v>
+      </c>
+      <c r="D18">
+        <v>2.1340000000000001E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19">
+        <v>0.20558999999999999</v>
+      </c>
+      <c r="D19">
+        <v>3.3860000000000001E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20">
+        <v>0.57589999999999997</v>
+      </c>
+      <c r="D20">
+        <v>3.32E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21">
+        <v>0.58130000000000004</v>
+      </c>
+      <c r="D21">
+        <v>0.1091</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>33</v>
+      </c>
+      <c r="C22">
+        <v>0.1198</v>
+      </c>
+      <c r="D22">
+        <v>5.1749999999999997E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24">
+        <v>0.99021999999999999</v>
+      </c>
+      <c r="D24">
+        <v>1.6590000000000001E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27">
+        <v>0.49404999999999999</v>
+      </c>
+      <c r="D27">
+        <v>4.7910000000000001E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>33</v>
+      </c>
+      <c r="C29">
+        <v>-0.24257000000000001</v>
+      </c>
+      <c r="D29">
+        <v>2.9749999999999999E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>37</v>
+      </c>
+      <c r="C31">
+        <v>0.59584000000000004</v>
+      </c>
+      <c r="D31">
+        <v>7.0620000000000002E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32">
+        <v>1.052019</v>
+      </c>
+      <c r="D32">
+        <v>4.182E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>33</v>
+      </c>
+      <c r="C33">
+        <v>-0.184</v>
+      </c>
+      <c r="D33">
+        <v>0.113</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34">
+        <v>-0.21190000000000001</v>
+      </c>
+      <c r="D34">
+        <v>5.5899999999999998E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03A81605-B8FD-4748-BBEB-9C956ABFBBB3}">
+  <dimension ref="A1:D34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2">
+        <v>0.92777699999999996</v>
+      </c>
+      <c r="D2">
+        <v>2.5219999999999999E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <v>0.82155</v>
+      </c>
+      <c r="D3">
+        <v>2.844E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4">
+        <v>1.0601499999999999</v>
+      </c>
+      <c r="D4">
+        <v>7.7999999999999996E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>0.51229999999999998</v>
+      </c>
+      <c r="D5">
+        <v>0.12239999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <v>0.56781999999999999</v>
+      </c>
+      <c r="D6">
+        <v>4.1660000000000003E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>0.76863000000000004</v>
+      </c>
+      <c r="D7">
+        <v>1.405E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8">
+        <v>1.128169</v>
+      </c>
+      <c r="D8">
+        <v>3.8279999999999998E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9">
+        <v>0.37845000000000001</v>
+      </c>
+      <c r="D9">
+        <v>8.7859999999999994E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10">
+        <v>0.17169999999999999</v>
+      </c>
+      <c r="D10">
+        <v>4.3770000000000003E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11">
+        <v>0.98675599999999997</v>
+      </c>
+      <c r="D11">
+        <v>8.3210000000000003E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12">
+        <v>1.0574399999999999</v>
+      </c>
+      <c r="D12">
+        <v>1.2149999999999999E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13">
+        <v>0.36599999999999999</v>
+      </c>
+      <c r="D13">
+        <v>5.6009999999999997E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{144686B2-EC4A-554B-A567-89EF351347AB}">
+  <dimension ref="A1:D34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">

</xml_diff>

<commit_message>
Added jobtypes in supporting docs
</commit_message>
<xml_diff>
--- a/Results/VisitFreqResults.xlsx
+++ b/Results/VisitFreqResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ellieodole/Desktop/CompEpi/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B5BF80B-3C8C-284F-8C2D-27F5514FC5DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45646264-77EA-9548-83C7-A5155D179949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12040" yWindow="500" windowWidth="16760" windowHeight="15800" firstSheet="3" activeTab="7" xr2:uid="{79939B0F-1E38-4E44-BCA6-B963B8C4AFB2}"/>
+    <workbookView xWindow="12040" yWindow="500" windowWidth="16760" windowHeight="15800" firstSheet="6" activeTab="9" xr2:uid="{79939B0F-1E38-4E44-BCA6-B963B8C4AFB2}"/>
   </bookViews>
   <sheets>
     <sheet name="GroupA Weekday" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,8 @@
     <sheet name="GroupC Weekend" sheetId="6" r:id="rId6"/>
     <sheet name="GroupD Weekday" sheetId="7" r:id="rId7"/>
     <sheet name="GroupD Weekend" sheetId="8" r:id="rId8"/>
-    <sheet name="Sheet2" sheetId="9" r:id="rId9"/>
+    <sheet name="Group E Weekday" sheetId="10" r:id="rId9"/>
+    <sheet name="GroupE Weekend" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="26">
   <si>
     <t>Job Type ID</t>
   </si>
@@ -93,6 +94,33 @@
   </si>
   <si>
     <t>33 42</t>
+  </si>
+  <si>
+    <t>19 20 24 25 43</t>
+  </si>
+  <si>
+    <t>19 20 24 25</t>
+  </si>
+  <si>
+    <t>20 24 25 43</t>
+  </si>
+  <si>
+    <t>19 20 25</t>
+  </si>
+  <si>
+    <t>19 20 24</t>
+  </si>
+  <si>
+    <t>19 24 25</t>
+  </si>
+  <si>
+    <t>19 24 43</t>
+  </si>
+  <si>
+    <t>19 24 25 43</t>
+  </si>
+  <si>
+    <t>19 24</t>
   </si>
 </sst>
 </file>
@@ -936,6 +964,272 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{885E34F6-CCE7-FE4A-B84B-2C27C3F8C661}">
+  <dimension ref="A1:D34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2">
+        <v>0.99772380000000005</v>
+      </c>
+      <c r="D2">
+        <v>7.6119999999999996E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3">
+        <v>0.79286599999999996</v>
+      </c>
+      <c r="D3">
+        <v>7.2439999999999996E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4">
+        <v>0.95370600000000005</v>
+      </c>
+      <c r="D4">
+        <v>0.29270000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5">
+        <v>0.26656000000000002</v>
+      </c>
+      <c r="D5">
+        <v>1.9369999999999998E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6">
+        <v>0.57762000000000002</v>
+      </c>
+      <c r="D6">
+        <v>1.1169999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7">
+        <v>0.55432899999999996</v>
+      </c>
+      <c r="D7">
+        <v>4.0460000000000001E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8">
+        <v>1.247296</v>
+      </c>
+      <c r="D8">
+        <v>1.2509999999999999E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9">
+        <v>0.30778</v>
+      </c>
+      <c r="D9">
+        <v>1.5970000000000002E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4746EA15-A9C7-214F-9C01-6BD036FBC0AB}">
   <dimension ref="A1:D34"/>
@@ -3604,8 +3898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03A81605-B8FD-4748-BBEB-9C956ABFBBB3}">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3796,105 +4090,294 @@
       <c r="A14">
         <v>13</v>
       </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>1.0887</v>
+      </c>
+      <c r="D14">
+        <v>1.3299999999999999E-2</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15">
+        <v>0.77548899999999998</v>
+      </c>
+      <c r="D15">
+        <v>9.7929999999999996E-3</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>0.2001</v>
+      </c>
+      <c r="D16">
+        <v>0.14510000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18">
+        <v>0.31595000000000001</v>
+      </c>
+      <c r="D18">
+        <v>5.8689999999999999E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19">
+        <v>-1.4255</v>
+      </c>
+      <c r="D19">
+        <v>0.56659999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <v>42</v>
+      </c>
+      <c r="C21">
+        <v>1.03725</v>
+      </c>
+      <c r="D21">
+        <v>0.9496</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <v>33</v>
+      </c>
+      <c r="C22">
+        <v>0.88329999999999997</v>
+      </c>
+      <c r="D22">
+        <v>0.13039999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24">
+        <v>1.4402600000000001</v>
+      </c>
+      <c r="D24">
+        <v>4.2639999999999997E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B29">
+        <v>33</v>
+      </c>
+      <c r="C29">
+        <v>-4.1799999999999997E-2</v>
+      </c>
+      <c r="D29">
+        <v>4.3400000000000001E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32">
+        <v>1.2733570000000001</v>
+      </c>
+      <c r="D32">
+        <v>7.4679999999999998E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34">
+        <v>-0.28170000000000001</v>
+      </c>
+      <c r="D34">
+        <v>0.25380000000000003</v>
       </c>
     </row>
   </sheetData>
@@ -3903,14 +4386,17 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{144686B2-EC4A-554B-A567-89EF351347AB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54DE3488-424E-474B-8CB5-B6F73C1973F2}">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D34"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -3930,165 +4416,462 @@
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2">
+        <v>0.98721362999999995</v>
+      </c>
+      <c r="D2">
+        <v>4.4569999999999999E-4</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3">
+        <v>0.71974700000000003</v>
+      </c>
+      <c r="D3">
+        <v>3.3470000000000001E-3</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4">
+        <v>0.94683499999999998</v>
+      </c>
+      <c r="D4">
+        <v>1.789E-3</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5">
+        <v>0.108336</v>
+      </c>
+      <c r="D5">
+        <v>6.5579999999999996E-3</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6">
+        <v>0.58696899999999996</v>
+      </c>
+      <c r="D6">
+        <v>4.7629999999999999E-3</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7">
+        <v>0.41144900000000001</v>
+      </c>
+      <c r="D7">
+        <v>2.4459999999999998E-3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8">
+        <v>1.2040465199999999</v>
+      </c>
+      <c r="D8">
+        <v>7.2753999999999996E-3</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9">
+        <v>0.25559500000000002</v>
+      </c>
+      <c r="D9">
+        <v>4.6730000000000001E-3</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10">
+        <v>0.1547</v>
+      </c>
+      <c r="D10">
+        <v>5.7340000000000004E-3</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11">
+        <v>0.96827700000000005</v>
+      </c>
+      <c r="D11">
+        <v>1.5900000000000001E-3</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12">
+        <v>0.824264</v>
+      </c>
+      <c r="D12">
+        <v>4.2360000000000002E-3</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13">
+        <v>0.42881999999999998</v>
+      </c>
+      <c r="D13">
+        <v>4.5519999999999996E-3</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14">
+        <v>1.104876</v>
+      </c>
+      <c r="D14">
+        <v>3.6150000000000002E-3</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15">
+        <v>0.40622999999999998</v>
+      </c>
+      <c r="D15">
+        <v>4.4600000000000004E-3</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16">
+        <v>6.9610000000000005E-2</v>
+      </c>
+      <c r="D16">
+        <v>1.013E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17">
+        <v>0.16450999999999999</v>
+      </c>
+      <c r="D17">
+        <v>3.7420000000000002E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>0.28161900000000001</v>
+      </c>
+      <c r="D18">
+        <v>5.4039999999999999E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19">
+        <v>0.22483</v>
+      </c>
+      <c r="D19">
+        <v>1.473E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20">
+        <v>0.12569</v>
+      </c>
+      <c r="D20">
+        <v>1.136E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21">
+        <v>0.86468699999999998</v>
+      </c>
+      <c r="D21">
+        <v>3.1470000000000001E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22">
+        <v>0.25785000000000002</v>
+      </c>
+      <c r="D22">
+        <v>1.055E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24">
+        <v>0.15196000000000001</v>
+      </c>
+      <c r="D24">
+        <v>1.038E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25">
+        <v>0.64299099999999998</v>
+      </c>
+      <c r="D25">
+        <v>3.4259999999999998E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27">
+        <v>0.43832599999999999</v>
+      </c>
+      <c r="D27">
+        <v>5.5310000000000003E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28">
+        <v>0.52037</v>
+      </c>
+      <c r="D28">
+        <v>1.0189999999999999E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B29">
+        <v>19</v>
+      </c>
+      <c r="C29">
+        <v>-0.67203999999999997</v>
+      </c>
+      <c r="D29">
+        <v>4.5069999999999999E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30">
+        <v>0.34189999999999998</v>
+      </c>
+      <c r="D30">
+        <v>1.324E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B31">
+        <v>19</v>
+      </c>
+      <c r="C31">
+        <v>0.87431899999999996</v>
+      </c>
+      <c r="D31">
+        <v>7.5269999999999998E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32">
+        <v>0.39977000000000001</v>
+      </c>
+      <c r="D32">
+        <v>5.79E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B33">
+        <v>25</v>
+      </c>
+      <c r="C33">
+        <v>0.88739000000000001</v>
+      </c>
+      <c r="D33">
+        <v>3.3860000000000001E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34">
+        <v>0.65878700000000001</v>
+      </c>
+      <c r="D34">
+        <v>3.1359999999999999E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished with visit freq results
</commit_message>
<xml_diff>
--- a/Results/VisitFreqResults.xlsx
+++ b/Results/VisitFreqResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ellieodole/Desktop/CompEpi/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A147AE2-D5CD-9545-96D7-FF49C0FF4CAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F681C040-6006-0C4E-8409-4824F9775158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12040" yWindow="500" windowWidth="16760" windowHeight="15800" firstSheet="9" activeTab="13" xr2:uid="{79939B0F-1E38-4E44-BCA6-B963B8C4AFB2}"/>
+    <workbookView xWindow="11740" yWindow="500" windowWidth="16760" windowHeight="15800" firstSheet="11" activeTab="15" xr2:uid="{79939B0F-1E38-4E44-BCA6-B963B8C4AFB2}"/>
   </bookViews>
   <sheets>
     <sheet name="GroupA Weekday" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,8 @@
     <sheet name="GroupF Weekend" sheetId="13" r:id="rId12"/>
     <sheet name="GroupG Weekday" sheetId="14" r:id="rId13"/>
     <sheet name="GroupG Weekend" sheetId="15" r:id="rId14"/>
+    <sheet name="GroupH Weekday" sheetId="16" r:id="rId15"/>
+    <sheet name="Sheet2" sheetId="17" r:id="rId16"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -47,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="37">
   <si>
     <t>Job Type ID</t>
   </si>
@@ -2684,8 +2686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C28FC6CE-858F-4E41-9B46-7622795EE6F0}">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2767,145 +2769,1385 @@
       <c r="B6" t="s">
         <v>36</v>
       </c>
+      <c r="C6">
+        <v>0.60906899999999997</v>
+      </c>
+      <c r="D6">
+        <v>9.2759999999999995E-3</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7">
+        <v>0.4975</v>
+      </c>
+      <c r="D7">
+        <v>7.4099999999999999E-3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8">
+        <v>1.31819</v>
+      </c>
+      <c r="D8">
+        <v>1.3010000000000001E-3</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9">
+        <v>0.46812999999999999</v>
+      </c>
+      <c r="D9">
+        <v>1.5339999999999999E-2</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10">
+        <v>0.69403999999999999</v>
+      </c>
+      <c r="D10">
+        <v>6.3210000000000002E-3</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11">
+        <v>1.019218</v>
+      </c>
+      <c r="D11">
+        <v>2.3587E-3</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12">
+        <v>1.2135</v>
+      </c>
+      <c r="D12">
+        <v>1.15E-2</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13">
+        <v>0.69882999999999995</v>
+      </c>
+      <c r="D13">
+        <v>7.2100000000000003E-3</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14">
+        <v>0.72526000000000002</v>
+      </c>
+      <c r="D14">
+        <v>1.155E-2</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15">
+        <v>0.4395</v>
+      </c>
+      <c r="D15">
+        <v>4.1050000000000003E-2</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16">
+        <v>0.51219000000000003</v>
+      </c>
+      <c r="D16">
+        <v>1.933E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18">
+        <v>0.64180700000000002</v>
+      </c>
+      <c r="D18">
+        <v>7.8009999999999998E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19">
+        <v>7.0129999999999998E-2</v>
+      </c>
+      <c r="D19">
+        <v>2.094E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>0.92854999999999999</v>
+      </c>
+      <c r="D20">
+        <v>2.3779999999999999E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22">
+        <v>0.66818</v>
+      </c>
+      <c r="D22">
+        <v>2.632E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24">
+        <v>0.20946999999999999</v>
+      </c>
+      <c r="D24">
+        <v>1.9130000000000001E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25">
+        <v>0.73709000000000002</v>
+      </c>
+      <c r="D25">
+        <v>1.9529999999999999E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26">
+        <v>1.2556529999999999</v>
+      </c>
+      <c r="D26">
+        <v>6.0590000000000001E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27">
+        <v>0.95845000000000002</v>
+      </c>
+      <c r="D27">
+        <v>1.932E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B28">
+        <v>16</v>
+      </c>
+      <c r="C28">
+        <v>0.52249999999999996</v>
+      </c>
+      <c r="D28">
+        <v>5.5E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29">
+        <v>1.0453600000000001</v>
+      </c>
+      <c r="D29">
+        <v>1.2460000000000001E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B30">
+        <v>16</v>
+      </c>
+      <c r="C30">
+        <v>0.53505999999999998</v>
+      </c>
+      <c r="D30">
+        <v>4.6940000000000003E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B31">
+        <v>9</v>
+      </c>
+      <c r="C31">
+        <v>-0.76739999999999997</v>
+      </c>
+      <c r="D31">
+        <v>0.36520000000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32">
+        <v>0.57932700000000004</v>
+      </c>
+      <c r="D32">
+        <v>5.2090000000000001E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34">
+        <v>0.72706099999999996</v>
+      </c>
+      <c r="D34">
+        <v>5.9829999999999996E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D2B04C5-66C6-A445-BC18-1E8FC6AF0C2F}">
+  <dimension ref="A1:D34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>0.98434379999999999</v>
+      </c>
+      <c r="D2">
+        <v>8.0380000000000002E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>0.65761599999999998</v>
+      </c>
+      <c r="D3">
+        <v>4.2090000000000001E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>1.1915629999999999</v>
+      </c>
+      <c r="D4">
+        <v>3.176E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>0.11072</v>
+      </c>
+      <c r="D5">
+        <v>1.383E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>0.73948499999999995</v>
+      </c>
+      <c r="D6">
+        <v>4.993E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>0.46534999999999999</v>
+      </c>
+      <c r="D7">
+        <v>2.5729999999999999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>1.1643619999999999</v>
+      </c>
+      <c r="D8">
+        <v>1.4959999999999999E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>0.60714800000000002</v>
+      </c>
+      <c r="D9">
+        <v>6.6610000000000003E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>1.5439E-2</v>
+      </c>
+      <c r="D10">
+        <v>9.1420000000000008E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>0.90307999999999999</v>
+      </c>
+      <c r="D11">
+        <v>3.0530000000000002E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>0.55544099999999996</v>
+      </c>
+      <c r="D13">
+        <v>6.7949999999999998E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>0.74112</v>
+      </c>
+      <c r="D14">
+        <v>1.119E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <v>0.22578000000000001</v>
+      </c>
+      <c r="D15">
+        <v>2.053E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>10</v>
+      </c>
+      <c r="C16">
+        <v>0.51239000000000001</v>
+      </c>
+      <c r="D16">
+        <v>9.1570000000000002E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>10</v>
+      </c>
+      <c r="C18">
+        <v>-0.51114000000000004</v>
+      </c>
+      <c r="D18">
+        <v>3.9620000000000002E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>10</v>
+      </c>
+      <c r="C20">
+        <v>0.68235999999999997</v>
+      </c>
+      <c r="D20">
+        <v>2.3259999999999999E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>10</v>
+      </c>
+      <c r="C22">
+        <v>-3.7249999999999998E-2</v>
+      </c>
+      <c r="D22">
+        <v>5.2699999999999997E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>10</v>
+      </c>
+      <c r="C25">
+        <v>0.40160000000000001</v>
+      </c>
+      <c r="D25">
+        <v>2.81E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>10</v>
+      </c>
+      <c r="C27">
+        <v>-0.15598999999999999</v>
+      </c>
+      <c r="D27">
+        <v>5.586E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>10</v>
+      </c>
+      <c r="C28">
+        <v>0.59174000000000004</v>
+      </c>
+      <c r="D28">
+        <v>1.0120000000000001E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>10</v>
+      </c>
+      <c r="C30">
+        <v>0.49127999999999999</v>
+      </c>
+      <c r="D30">
+        <v>1.014E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>10</v>
+      </c>
+      <c r="C33">
+        <v>0.33337</v>
+      </c>
+      <c r="D33">
+        <v>5.323E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>10</v>
+      </c>
+      <c r="C34">
+        <v>7.7939999999999995E-2</v>
+      </c>
+      <c r="D34">
+        <v>4.6620000000000002E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80F0CCE1-6112-F149-B5ED-8369A940BB07}">
+  <dimension ref="A1:D34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>0.992228</v>
+      </c>
+      <c r="D2">
+        <v>1.467E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>0.62439</v>
+      </c>
+      <c r="D3">
+        <v>1.0919999999999999E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>1.2150749999999999</v>
+      </c>
+      <c r="D4">
+        <v>5.1250000000000002E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>0.11777</v>
+      </c>
+      <c r="D5">
+        <v>5.842E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>0.71723000000000003</v>
+      </c>
+      <c r="D6">
+        <v>1.418E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>0.50863000000000003</v>
+      </c>
+      <c r="D7">
+        <v>4.342E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>1.1623270000000001</v>
+      </c>
+      <c r="D8">
+        <v>2.8960000000000001E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>0.98094999999999999</v>
+      </c>
+      <c r="D9">
+        <v>1.409E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>-8.8959999999999997E-2</v>
+      </c>
+      <c r="D10">
+        <v>2.2360000000000001E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>0.93836900000000001</v>
+      </c>
+      <c r="D11">
+        <v>6.1619999999999999E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>0.56777</v>
+      </c>
+      <c r="D13">
+        <v>1.9460000000000002E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>0.75048000000000004</v>
+      </c>
+      <c r="D14">
+        <v>2.1489999999999999E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <v>0.21029999999999999</v>
+      </c>
+      <c r="D15">
+        <v>3.4959999999999998E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>10</v>
+      </c>
+      <c r="C16">
+        <v>0.46779999999999999</v>
+      </c>
+      <c r="D16">
+        <v>2.4199999999999999E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>10</v>
+      </c>
+      <c r="C18">
+        <v>-0.43117</v>
+      </c>
+      <c r="D18">
+        <v>6.2509999999999996E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>10</v>
+      </c>
+      <c r="C20">
+        <v>-0.12230000000000001</v>
+      </c>
+      <c r="D20">
+        <v>0.15509999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>10</v>
+      </c>
+      <c r="C22">
+        <v>-0.36073</v>
+      </c>
+      <c r="D22">
+        <v>3.8190000000000002E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>10</v>
+      </c>
+      <c r="C25">
+        <v>0.39578000000000002</v>
+      </c>
+      <c r="D25">
+        <v>5.3159999999999999E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>10</v>
+      </c>
+      <c r="C27">
+        <v>1.0097</v>
+      </c>
+      <c r="D27">
+        <v>0.16739999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>10</v>
+      </c>
+      <c r="C28">
+        <v>0.33448</v>
+      </c>
+      <c r="D28">
+        <v>5.6410000000000002E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>10</v>
+      </c>
+      <c r="C30">
+        <v>0.88739000000000001</v>
+      </c>
+      <c r="D30">
+        <v>1.9570000000000001E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>10</v>
+      </c>
+      <c r="C34">
+        <v>0.52829999999999999</v>
+      </c>
+      <c r="D34">
+        <v>0.17299999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update to organization of repo
</commit_message>
<xml_diff>
--- a/Results/VisitFreqResults.xlsx
+++ b/Results/VisitFreqResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ellieodole/Desktop/CompEpi/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F681C040-6006-0C4E-8409-4824F9775158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B831ED-4C93-1C48-901B-626FB6A187C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11740" yWindow="500" windowWidth="16760" windowHeight="15800" firstSheet="11" activeTab="15" xr2:uid="{79939B0F-1E38-4E44-BCA6-B963B8C4AFB2}"/>
   </bookViews>
@@ -28,7 +28,7 @@
     <sheet name="GroupG Weekday" sheetId="14" r:id="rId13"/>
     <sheet name="GroupG Weekend" sheetId="15" r:id="rId14"/>
     <sheet name="GroupH Weekday" sheetId="16" r:id="rId15"/>
-    <sheet name="Sheet2" sheetId="17" r:id="rId16"/>
+    <sheet name="GroupH Weekend" sheetId="17" r:id="rId16"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -3669,7 +3669,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>